<commit_message>
LL table update, doc update
</commit_message>
<xml_diff>
--- a/documentation/Gramatika-ver08.xlsx
+++ b/documentation/Gramatika-ver08.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\_EVA\FIT\2021-LS\IVS\project02\addingToGithub\IFJ21\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3efae75f706e1dc0/_EVA/FIT/2021-LS/IVS/project02/addingToGithub/IFJ21/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB3D9DF-E84E-4E04-97CD-B3A1C9A08414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{E532FE7A-99BD-40E5-997B-EE05DA8802FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15330" yWindow="8220" windowWidth="28800" windowHeight="15465" xr2:uid="{F7ABA761-DE8C-46A3-9A12-1AE5C5993C9B}"/>
+    <workbookView xWindow="-45735" yWindow="11340" windowWidth="19200" windowHeight="10305" xr2:uid="{F7ABA761-DE8C-46A3-9A12-1AE5C5993C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -691,9 +691,7 @@
   </sheetPr>
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
LL table repaired, new test added
</commit_message>
<xml_diff>
--- a/documentation/Gramatika-ver08.xlsx
+++ b/documentation/Gramatika-ver08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3efae75f706e1dc0/_EVA/FIT/2021-LS/IVS/project02/addingToGithub/IFJ21/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E532FE7A-99BD-40E5-997B-EE05DA8802FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{E532FE7A-99BD-40E5-997B-EE05DA8802FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A7E6A5C-119B-472D-A9CB-9F02AFE8E67D}"/>
   <bookViews>
-    <workbookView xWindow="-45735" yWindow="11340" windowWidth="19200" windowHeight="10305" xr2:uid="{F7ABA761-DE8C-46A3-9A12-1AE5C5993C9B}"/>
+    <workbookView xWindow="-45225" yWindow="11850" windowWidth="19200" windowHeight="10305" xr2:uid="{F7ABA761-DE8C-46A3-9A12-1AE5C5993C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -252,9 +252,6 @@
     <t>function id_f ( &lt;params_list&gt; &lt;return_fc&gt; end &lt;prog&gt;</t>
   </si>
   <si>
-    <t>epsilon</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;expressions&gt; </t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>number_int_value</t>
+  </si>
+  <si>
+    <t>Ԑ</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +371,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,7 +694,9 @@
   </sheetPr>
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -924,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1190,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1204,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1212,7 +1217,7 @@
         <v>37.1</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>1</v>
@@ -1226,13 +1231,13 @@
         <v>37.200000000000003</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1240,13 +1245,13 @@
         <v>37.299999999999997</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1254,13 +1259,13 @@
         <v>37.4</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1268,13 +1273,13 @@
         <v>37.5</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1301,8 +1306,8 @@
       <c r="C44" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>72</v>
+      <c r="D44" s="14" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1590,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>